<commit_message>
add new examples to table
</commit_message>
<xml_diff>
--- a/survey_experiments_literature.xlsx
+++ b/survey_experiments_literature.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cord/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cord/Documents/GitHub/survey_experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{EDD3B6B5-C707-1F44-9F5C-A45CAE210A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE8C2B3-5386-CB44-B4A0-8E837E901DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9900" yWindow="-28140" windowWidth="50880" windowHeight="27980" xr2:uid="{AC52B365-6B50-0648-94BA-0E6BB0E06CDD}"/>
+    <workbookView xWindow="-10060" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{AC52B365-6B50-0648-94BA-0E6BB0E06CDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Frederiksen, K., &amp; Laustsen, L. (2025). Interstate Conflict Increases the Appeal of Undemocratic Candidates. British Journal of Political Science, 55, e138. doi:10.1017/S0007123425101014</t>
   </si>
@@ -61,12 +60,6 @@
   </si>
   <si>
     <t>authors, study, journal</t>
-  </si>
-  <si>
-    <t>- study 1, no; see interpretation:
-    - *„In support of our argument, Figure 1 shows that undemocratic candidates are perceived as 20 percentage points more dominant than democratically compliant candidates.“ (Frederiksen und Laustsen, 2025, p. 4)
-- study 2, no:
-    - „we find that an undemocratic presidential candidate is strongly disfavored during peace, but that the relative appeal of democraticness is significantly reduced when threats of interstate conflict appear. Respondents still prefer a democratic candidate during conflict, but recall that this is when party is held constant.“ (Frederiksen und Laustsen, 2025, p. 6)</t>
   </si>
   <si>
     <t>- reference to “roubstness” for inclusion of controls in study 1:
@@ -78,13 +71,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- study 1: decscriptive estimand; mean preferences for politicians personality traits;
-- study 2: descriptive estimand; mean preferences for politicians personality traits across three different survey set-ups;
-- study 3: AMCE, thus descpriptive (?): the wording implies that they want to to determine the causal effect of politicians personalities and characteristics on voter preferences (choice for one of two candidate profiles); „We estimate average marginal component effects (AMCEs) to identify the effect of the different attributes on our dependent variable“ (p. 11) 
-  „The AMCEs are presented in Figure 4. The points represent the estimates by country, and the bars represent the 95% confidence intervals. These estimates can be interpreted as the effect of each attribute level (relative to that attribute's reference category) on citizens' probability of selecting a candidate, averaged across all possible combinations of other attributes (Abramson et al., 2019; Bansak et al., 2020).“ (p. 12)
-    - *„Study 3 extends this work using an experimental approach (conjoint experiment), allowing for the estimation of the causal effect of politicians' personalities on voter preferences as well as the causal effects of other individual characteristics of elites.“ (p. 9) </t>
   </si>
   <si>
     <t xml:space="preserve">motivation for inclusion of attributes: real-world vs accountability  </t>
@@ -148,22 +134,12 @@
     <t xml:space="preserve">unclear: they talk about conjoints to uncover effects on choices: "Respondents are provided with multiple reasons to justify any particular choice (Hainmueller et al., 2014). Choices also do not require assessments of absolute levels of corruption, political services, or work motivation—only relative assessments of two choices." (p. 766) </t>
   </si>
   <si>
-    <t>- study 1 and 2: no;
-- in study 3, they use AMCE as estimator, de-facto inferential target is thus descriptive? yet they talk about casual effects: [@[justification of controls]]
-„Study 3 extends this work using an experimental approach (conjoint experiment), allowing for the estimation of the causal effect of politicians' personalities on voter preferences as well as the causal effects of other individual characteristics of elites.“</t>
-  </si>
-  <si>
     <t>- in study 1 and 2, no reference to controls; 
 -  in study 3: "We also neutralize the confounding effect of ideology and partisan sorting by investigating within-party leader preferences (Study 3). With this design, we create a hypothetical environment where we control for ideology, estimating a more realistic effect of personality on preferences“ (p. 3)</t>
   </si>
   <si>
     <t>- in study 2, they talk about their results as real world scenarios: 
 „Supporting our argument, we find that an undemocratic presidential candidate is strongly disfavored during peace, but that the relative appeal of democraticness is significantly reduced when threats of interstate conflict appear.“ (p. 6)</t>
-  </si>
-  <si>
-    <t>Study 1 : descriptive - they measure how the (information about) undemocratic behavior of candidates affects their dominance impression on behalf of the participants „Specifically, we randomly assigned undemocratic and democratic behaviors – along with background attributes, policy positions, and party – to potential future candidates in gubernatorial elections and measured how the respondents perceived these candidates in terms of dominance.“ (Frederiksen und Laustsen, 2025, p. 3)
-- Study 2: descriptive - they compare how effects of information about undemocratic behavior on candidate appeal (rated capability and reported vote intentions) differs given primes about security scenarios (peace vs conflict);  
-  „We fielded a factorial vignette experiment (N = 2,611 respondents meeting census-based quotas on gender, age, region, and education) with YouGov in December 2023 to test whether the appeal of undemocratic candidates is amplified during threats of interstate conflict.“* (Frederiksen und Laustsen, 2025, p. 4)</t>
   </si>
   <si>
     <t xml:space="preserve">bib handle </t>
@@ -199,6 +175,155 @@
   year={2018},
   publisher={SAGE Publications Sage CA: Los Angeles, CA}
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- hypothesis 1: -&gt; descriptive 
+- hypothesis 2: -&gt; unclear, but set-up implies descriptive estimand, although they report treatment effects; 
+- hypothesis 3: -&gt; descriptive 
+- hypothesis 4: -&gt; descriptive </t>
+  </si>
+  <si>
+    <t>- for Hypothesis 1, they report the average difference of affective polarization between conditions (convergent vs divergent ideological position of hypothetical candidates), thus, descriptive estimand; however their refer to results as effects: 
+"Thus, ideological divergence affected evaluations of both candidates, where respondents in the divergent condition gave more positive ratings to the more proximate candidate and more negative ratings to the opponent.“ (p. 494)
+- for Hypothesis 2, they compare "effects" found in Hypothesis 1 and refer to them as treatment effects: 
+"To test this hypothesis, we compare the effects of divergence based on respondents’ self-reported ideological locations." (p. 495) 
+"Figure 3 displays the treatment effect of candidate divergence (the difference in means in affective polarization) for respondents at each point on the ideological scale." (p. 495)
+- for hypothesis 3, they compare levels of affective polarization between high and low levels of political interest; however, they also take about comparison of effects in this regard:
+ „Our third hypothesis posits that the effects of ideological divergence are greater among individuals with higher levels of political interest, who may be especially likely to engage in motivated reasoning to support their preferred candidate. To test this hypothesis, we distinguish respondents based on their reported levels of political interest.16 Prior to receiving the treatment, respondents were asked to indicate their level of interest ‘‘about what’s going on in government and politics.’’ We compare the effects of ideological divergence among respondents who were ‘‘extremely interested’’ or ‘‘very interested’’ (N = 889) to the effects among respondents who reported lower levels of interest (N = 828).17“ (p. 496)
+- hypothesis 4: comparison of effect found in H1 between respondents who received biographical information on candidates and those who did not, reported as treatment effects;
+„Among respondents who received only the candidates’ ideological locations, the mean level of affective polarization with the convergent candidates was 16.5 thermometer points (SE = 1.1), compared with 34.7 points (SE = 1.8) among respondents who were presented with the divergent candidates. Thus, the treatment effect of ideological divergence in the absence of additional information is 18.2 feeling thermometer points (SE = 2.2). Among respondents who also received biographical information about the candidates, the mean level of affective polarization with the convergent candidates was 19.6 (SE = 1.2), and 24.7 (SE = 1.6) among respondents with the divergent candidates. Thus, the treatment effect among respondents who received the information about the candidates’ backgrounds and personal lives was 5.1 feeling thermometer points (SE = 2.0).“ (p. 498)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no justification of controls; </t>
+  </si>
+  <si>
+    <t>- yes:
+„First, we demonstrate that citizens are quite responsive to ideology, and ideological extremity in particular. Citizens form affective evaluations of candidates and politicians on the basis of their ideological positions. When candidates or officeholders exhibit similar ideologies, citizens evaluate them similarly. However, as their ideological positions diverge, citizens express more divergent affective opinions about them. Thus, just as voters appear to choose presidential (Jessee 2009) and congressional (Shor and Rogowski forthcoming) candidates on the basis of ideological proximity, the results shown here contribute new evidence about other ways in which ideology affects political judgment.“ (p. 504) 
+- in the discussion, they refer to their results as causal evidence:
+„The results shown here build upon the findings in Abramowitz and Webster (2015) and Iyengar et al. (2012), who show that affective polarization towards elites and political parties has increased over time. Our experimental results provide causal evidence of this relationship, and our supplementary analysis of attitudes toward U.S. Senators suggests that these relationships extend to evaluations of individual officeholders.“ (p. 504)</t>
+  </si>
+  <si>
+    <t>Rogowski, J. C., &amp; Sutherland, J. L. (2016). How ideology fuels affective polarization. Political behavior, 38(2), 485-508.</t>
+  </si>
+  <si>
+    <t>@article{rogowski2016ideology,
+  title={How ideology fuels affective polarization},
+  author={Rogowski, Jon C and Sutherland, Joseph L},
+  journal={Political behavior},
+  volume={38},
+  number={2},
+  pages={485--508},
+  year={2016},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survey experiment, type not stated explicitly; </t>
+  </si>
+  <si>
+    <t>vignette experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- descriptive estimand: difference in average levels of dehumanization of in- and out-partisans given vignette that displays negative image of democrat/republican party event (p. 532) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- could be read as effect of real world features/outcomes: 
+"Our experimental results also shed new light on the potential underlying causal mechanisms behind this phenomenon." (p. 519) 
+"We find that Republicans are marginally more likely to dehumanize the perpetrators than Democrats overall." (p 534) </t>
+  </si>
+  <si>
+    <t>Martherus, J. L., Martinez, A. G., Piff, P. K., &amp; Theodoridis, A. G. (2021). Party animals? Extreme partisan polarization and dehumanization. Political Behavior, 43(2), 517-540.</t>
+  </si>
+  <si>
+    <t>@article{martherus2021party,
+  title={Party animals? Extreme partisan polarization and dehumanization},
+  author={Martherus, James L and Martinez, Andres G and Piff, Paul K and Theodoridis, Alexander G},
+  journal={Political Behavior},
+  volume={43},
+  number={2},
+  pages={517--540},
+  year={2021},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t>- causal estimand: 
+"We therefore offer the preregistered hypothesis that exposure to rhetoric challenging election legitimacy will decrease respect for electoral norms and trust and confidence in elections relative to rhetoric that does not violate democratic norms, especially as exposure increases over time (H1)."</t>
+  </si>
+  <si>
+    <t>survey experiment, not explicitly stated;</t>
+  </si>
+  <si>
+    <t>- at one point, it could be understood this way:
+„As the figure indicates, Trump’s election norm violations decrease trust and confidence in elections among people who approve of him by 0.24 standard deviations, on average, across waves (P &lt; 0.005).“ (p. 3)
+- however, the authors also emphasize the lack of external validity of their findings:
+ „Caution is required in extrapolating these findings beyond the bounds of the survey context in which they were measured (a caveat we return to and expand upon in Conclusion).“ (p. 5)</t>
+  </si>
+  <si>
+    <t>- reference to inclusion of “prognostic covariates” listed in pre-registration (first wave outcomes, education, age, gender, region, party, ideology, knowledge, ethnicity); 
+- no explicit justification of controls;
+„Each model includes a set of prognostic covariates chosen using a lasso variable selection procedure (see preregistration for details) and fixed effects for the blocks from our block randomization procedure.“ (p. 3)</t>
+  </si>
+  <si>
+    <t>Clayton, K., Davis, N. T., Nyhan, B., Porter, E., Ryan, T. J., &amp; Wood, T. J. (2021). Elite rhetoric can undermine democratic norms. Proceedings of the National Academy of Sciences, 118(23), e2024125118.</t>
+  </si>
+  <si>
+    <t>@article{clayton2021elite,
+  title={Elite rhetoric can undermine democratic norms},
+  author={Clayton, Katherine and Davis, Nicholas T and Nyhan, Brendan and Porter, Ethan and Ryan, Timothy J and Wood, Thomas J},
+  journal={Proceedings of the National Academy of Sciences},
+  volume={118},
+  number={23},
+  pages={e2024125118},
+  year={2021},
+  publisher={National Academy of Sciences}
+}</t>
+  </si>
+  <si>
+    <t>- covariates are included in the analysis models for of all three studies, however the authors do not explicitly justify their inclusion for the models in all three studies;
+    - covariates: baseline outcomes, age, gender, ideology, party ID, race, education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- causal estimand: ANTE/APTE - average negative/positive treatment effects (p. 1500) </t>
+  </si>
+  <si>
+    <t>Guess, A., &amp; Coppock, A. (2020). Does counter-attitudinal information cause backlash? Results from three large survey experiments. British Journal of Political Science, 50(4), 1497-1515.</t>
+  </si>
+  <si>
+    <t>@article{guess2020does,
+  title={Does counter-attitudinal information cause backlash? Results from three large survey experiments},
+  author={Guess, Andrew and Coppock, Alexander},
+  journal={British Journal of Political Science},
+  volume={50},
+  number={4},
+  pages={1497--1515},
+  year={2020},
+  publisher={Cambridge University Press}
+}</t>
+  </si>
+  <si>
+    <t>Study 1 : descriptive - they measure how the (information about) undemocratic behavior of candidates affects their dominance impression on behalf of the participants: 
+„Specifically, we randomly assigned undemocratic and democratic behaviors – along with background attributes, policy positions, and party – to potential future candidates in gubernatorial elections and measured how the respondents perceived these candidates in terms of dominance.“ (p. 3)
+- Study 2: descriptive - they compare how effects of information about undemocratic behavior on candidate appeal (rated capability and reported vote intentions) differs given primes about security scenarios (peace vs conflict);  
+ „We fielded a factorial vignette experiment (N = 2,611 respondents meeting census-based quotas on gender, age, region, and education) with YouGov in December 2023 to test whether the appeal of undemocratic candidates is amplified during threats of interstate conflict.“*  (p. 4)</t>
+  </si>
+  <si>
+    <t>- study 1, no; see interpretation:
+    - *„In support of our argument, Figure 1 shows that undemocratic candidates are perceived as 20 percentage points more dominant than democratically compliant candidates.“ (p. 4)
+- study 2, no:
+    - „we find that an undemocratic presidential candidate is strongly disfavored during peace, but that the relative appeal of democraticness is significantly reduced when threats of interstate conflict appear. Respondents still prefer a democratic candidate during conflict, but recall that this is when party is held constant.“ (p. 6)</t>
+  </si>
+  <si>
+    <t>- study 1 and 2: no;
+- in study 3, they use AMCE as estimator, de-facto inferential target is thus descriptive? yet they talk about casual effects:
+„Study 3 extends this work using an experimental approach (conjoint experiment), allowing for the estimation of the causal effect of politicians' personalities on voter preferences as well as the causal effects of other individual characteristics of elites.“ (p. 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- study 1: decscriptive estimand; mean preferences for politicians personality traits;
+- study 2: descriptive estimand; mean preferences for politicians personality traits across three different survey set-ups;
+- study 3: AMCE, thus descpriptive (?): the wording implies that they want to to determine the causal effect of politicians personalities and characteristics on voter preferences (choice for one of two candidate profiles); „We estimate average marginal component effects (AMCEs) to identify the effect of the different attributes on our dependent variable“ (p. 11) 
+„The AMCEs are presented in Figure 4. The points represent the estimates by country, and the bars represent the 95% confidence intervals. These estimates can be interpreted as the effect of each attribute level (relative to that attribute's reference category) on citizens' probability of selecting a candidate, averaged across all possible combinations of other attributes (Abramson et al., 2019; Bansak et al., 2020).“ (p. 12)
+ „Study 3 extends this work using an experimental approach (conjoint experiment), allowing for the estimation of the causal effect of politicians' personalities on voter preferences as well as the causal effects of other individual characteristics of elites.“ (p. 9) </t>
   </si>
 </sst>
 </file>
@@ -335,10 +460,22 @@
   <dxfs count="16">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -355,35 +492,23 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -411,23 +536,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27066089-46C9-B34E-A09E-A04418AAE794}" name="Tabelle1" displayName="Tabelle1" ref="A1:N9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27066089-46C9-B34E-A09E-A04418AAE794}" name="Tabelle1" displayName="Tabelle1" ref="A1:N9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:N9" xr:uid="{27066089-46C9-B34E-A09E-A04418AAE794}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{FA8A15F2-7205-E04A-B427-46C32E23B541}" name="authors, study, journal" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{98817F0C-1C2C-6B40-969E-440F13300A5C}" name="bib handle " dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{40676CA9-4A6B-1E42-9F85-32E6487CB7DB}" name="Survey type" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3C9E7D71-5412-8D41-A7FF-F392F6908FD8}" name="Estimand" dataDxfId="6" dataCellStyle="20 % - Akzent3"/>
-    <tableColumn id="4" xr3:uid="{F48015FF-E47C-3441-807C-D12299126F81}" name="difference wording estimand/de-facto inferential targt" dataDxfId="4" dataCellStyle="20 % - Akzent3"/>
-    <tableColumn id="5" xr3:uid="{369CF0DB-C37E-324B-8823-94A2BAFFD566}" name="justification of controls" dataDxfId="3" dataCellStyle="20 % - Akzent2"/>
-    <tableColumn id="6" xr3:uid="{303F7BD1-2E1A-9B4B-A6E4-D22EF82ED0E2}" name="controls: reference to confounding" dataDxfId="2" dataCellStyle="20 % - Akzent2"/>
-    <tableColumn id="7" xr3:uid="{4C452212-A6BF-E94A-9A65-B9F6721473E3}" name="controls: precision argument at intervention stage/ controlled effect, with factors downstream to intervention; " dataDxfId="1" dataCellStyle="20 % - Akzent2"/>
-    <tableColumn id="8" xr3:uid="{F7AB6DF0-C958-4042-9109-673735D8D15B}" name="Effects: of real-world features on outcomes" dataDxfId="13" dataCellStyle="20 % - Akzent5"/>
-    <tableColumn id="9" xr3:uid="{6A4A63A4-6F4D-4D4C-9DE9-8F5948FF101C}" name="reference to attributes of units as causes? " dataDxfId="12" dataCellStyle="20 % - Akzent5"/>
-    <tableColumn id="13" xr3:uid="{486980BE-A9EF-6A4D-8D03-C3ACAD34119F}" name="reference to information as attributes" dataDxfId="11" dataCellStyle="20 % - Akzent5"/>
-    <tableColumn id="12" xr3:uid="{5CFC487D-ACF9-B641-9540-80EADDAF94B5}" name="reference to effects on respondents answers as effect on choices" dataDxfId="10" dataCellStyle="20 % - Akzent5"/>
-    <tableColumn id="10" xr3:uid="{6E33FF6C-E3A8-A342-A72A-91DAF1FDCDF0}" name="justification of inlcusion of attributes" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C6D8AC0B-C5D5-374F-A16B-D1C6F192FBD4}" name="motivation for inclusion of attributes: real-world vs accountability  " dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{FA8A15F2-7205-E04A-B427-46C32E23B541}" name="authors, study, journal" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{98817F0C-1C2C-6B40-969E-440F13300A5C}" name="bib handle " dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{40676CA9-4A6B-1E42-9F85-32E6487CB7DB}" name="Survey type" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3C9E7D71-5412-8D41-A7FF-F392F6908FD8}" name="Estimand" dataDxfId="10" dataCellStyle="20 % - Akzent3"/>
+    <tableColumn id="4" xr3:uid="{F48015FF-E47C-3441-807C-D12299126F81}" name="difference wording estimand/de-facto inferential targt" dataDxfId="9" dataCellStyle="20 % - Akzent3"/>
+    <tableColumn id="5" xr3:uid="{369CF0DB-C37E-324B-8823-94A2BAFFD566}" name="justification of controls" dataDxfId="8" dataCellStyle="20 % - Akzent2"/>
+    <tableColumn id="6" xr3:uid="{303F7BD1-2E1A-9B4B-A6E4-D22EF82ED0E2}" name="controls: reference to confounding" dataDxfId="7" dataCellStyle="20 % - Akzent2"/>
+    <tableColumn id="7" xr3:uid="{4C452212-A6BF-E94A-9A65-B9F6721473E3}" name="controls: precision argument at intervention stage/ controlled effect, with factors downstream to intervention; " dataDxfId="6" dataCellStyle="20 % - Akzent2"/>
+    <tableColumn id="8" xr3:uid="{F7AB6DF0-C958-4042-9109-673735D8D15B}" name="Effects: of real-world features on outcomes" dataDxfId="5" dataCellStyle="20 % - Akzent5"/>
+    <tableColumn id="9" xr3:uid="{6A4A63A4-6F4D-4D4C-9DE9-8F5948FF101C}" name="reference to attributes of units as causes? " dataDxfId="4" dataCellStyle="20 % - Akzent5"/>
+    <tableColumn id="13" xr3:uid="{486980BE-A9EF-6A4D-8D03-C3ACAD34119F}" name="reference to information as attributes" dataDxfId="3" dataCellStyle="20 % - Akzent5"/>
+    <tableColumn id="12" xr3:uid="{5CFC487D-ACF9-B641-9540-80EADDAF94B5}" name="reference to effects on respondents answers as effect on choices" dataDxfId="2" dataCellStyle="20 % - Akzent5"/>
+    <tableColumn id="10" xr3:uid="{6E33FF6C-E3A8-A342-A72A-91DAF1FDCDF0}" name="justification of inlcusion of attributes" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C6D8AC0B-C5D5-374F-A16B-D1C6F192FBD4}" name="motivation for inclusion of attributes: real-world vs accountability  " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB675B15-7CCC-1C4B-A7B8-324BE461B480}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,10 +901,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -791,28 +916,28 @@
         <v>4</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
@@ -820,176 +945,222 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
+    <row r="5" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
+    <row r="6" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
+    <row r="8" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="E8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="6"/>

</xml_diff>